<commit_message>
add adder --refresh issue
</commit_message>
<xml_diff>
--- a/excelhere/test.xlsx
+++ b/excelhere/test.xlsx
@@ -408,13 +408,13 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G40"/>
+  <dimension ref="A1:G74"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="I7" sqref="I7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="13.5"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="13.5" outlineLevelCol="0"/>
   <cols>
     <col width="3.5" bestFit="1" customWidth="1" style="1" min="1" max="1"/>
     <col width="9" customWidth="1" style="1" min="2" max="2"/>
@@ -486,10 +486,7 @@
       <c r="F2" s="0" t="n">
         <v>0</v>
       </c>
-      <c r="G2" s="1">
-        <f>F2*E2</f>
-        <v/>
-      </c>
+      <c r="G2" s="1" t="n"/>
     </row>
     <row r="3">
       <c r="A3" s="1" t="n">
@@ -516,10 +513,7 @@
       <c r="F3" s="0" t="n">
         <v>0</v>
       </c>
-      <c r="G3" s="1">
-        <f>F3*E3</f>
-        <v/>
-      </c>
+      <c r="G3" s="1" t="n"/>
     </row>
     <row r="4">
       <c r="A4" s="1" t="n">
@@ -546,10 +540,7 @@
       <c r="F4" s="0" t="n">
         <v>0</v>
       </c>
-      <c r="G4" s="1">
-        <f>F4*E4</f>
-        <v/>
-      </c>
+      <c r="G4" s="1" t="n"/>
     </row>
     <row r="5">
       <c r="A5" s="1" t="n">
@@ -576,10 +567,7 @@
       <c r="F5" s="0" t="n">
         <v>0</v>
       </c>
-      <c r="G5" s="1">
-        <f>F5*E5</f>
-        <v/>
-      </c>
+      <c r="G5" s="1" t="n"/>
     </row>
     <row r="6">
       <c r="A6" s="1" t="n">
@@ -606,10 +594,7 @@
       <c r="F6" s="0" t="n">
         <v>0</v>
       </c>
-      <c r="G6" s="1">
-        <f>F6*E6</f>
-        <v/>
-      </c>
+      <c r="G6" s="1" t="n"/>
     </row>
     <row r="7">
       <c r="A7" s="1" t="n">
@@ -636,10 +621,7 @@
       <c r="F7" s="0" t="n">
         <v>0</v>
       </c>
-      <c r="G7" s="1">
-        <f>F7*E7</f>
-        <v/>
-      </c>
+      <c r="G7" s="1" t="n"/>
     </row>
     <row r="8">
       <c r="A8" s="1" t="n">
@@ -666,10 +648,7 @@
       <c r="F8" s="0" t="n">
         <v>0</v>
       </c>
-      <c r="G8" s="1">
-        <f>F8*E8</f>
-        <v/>
-      </c>
+      <c r="G8" s="1" t="n"/>
     </row>
     <row r="9">
       <c r="A9" s="1" t="n">
@@ -696,10 +675,7 @@
       <c r="F9" s="0" t="n">
         <v>0</v>
       </c>
-      <c r="G9" s="1">
-        <f>F9*E9</f>
-        <v/>
-      </c>
+      <c r="G9" s="1" t="n"/>
     </row>
     <row r="10">
       <c r="A10" s="1" t="n">
@@ -726,10 +702,7 @@
       <c r="F10" s="0" t="n">
         <v>0</v>
       </c>
-      <c r="G10" s="1">
-        <f>F10*E10</f>
-        <v/>
-      </c>
+      <c r="G10" s="1" t="n"/>
     </row>
     <row r="11">
       <c r="A11" s="1" t="n">
@@ -756,10 +729,7 @@
       <c r="F11" s="0" t="n">
         <v>0</v>
       </c>
-      <c r="G11" s="1">
-        <f>F11*E11</f>
-        <v/>
-      </c>
+      <c r="G11" s="1" t="n"/>
     </row>
     <row r="12">
       <c r="A12" s="1" t="n">
@@ -786,10 +756,7 @@
       <c r="F12" s="0" t="n">
         <v>0</v>
       </c>
-      <c r="G12" s="1">
-        <f>F12*E12</f>
-        <v/>
-      </c>
+      <c r="G12" s="1" t="n"/>
     </row>
     <row r="13">
       <c r="A13" s="1" t="n">
@@ -816,10 +783,7 @@
       <c r="F13" s="0" t="n">
         <v>0</v>
       </c>
-      <c r="G13" s="1">
-        <f>F13*E13</f>
-        <v/>
-      </c>
+      <c r="G13" s="1" t="n"/>
     </row>
     <row r="14">
       <c r="A14" s="1" t="n">
@@ -846,10 +810,7 @@
       <c r="F14" s="0" t="n">
         <v>0</v>
       </c>
-      <c r="G14" s="1">
-        <f>F14*E14</f>
-        <v/>
-      </c>
+      <c r="G14" s="1" t="n"/>
     </row>
     <row r="15">
       <c r="A15" s="1" t="n">
@@ -876,10 +837,7 @@
       <c r="F15" s="0" t="n">
         <v>0</v>
       </c>
-      <c r="G15" s="1">
-        <f>F15*E15</f>
-        <v/>
-      </c>
+      <c r="G15" s="1" t="n"/>
     </row>
     <row r="16">
       <c r="A16" s="1" t="n">
@@ -906,10 +864,7 @@
       <c r="F16" s="0" t="n">
         <v>0</v>
       </c>
-      <c r="G16" s="1">
-        <f>F16*E16</f>
-        <v/>
-      </c>
+      <c r="G16" s="1" t="n"/>
     </row>
     <row r="17">
       <c r="A17" s="1" t="n">
@@ -936,10 +891,7 @@
       <c r="F17" s="0" t="n">
         <v>0</v>
       </c>
-      <c r="G17" s="1">
-        <f>F17*E17</f>
-        <v/>
-      </c>
+      <c r="G17" s="1" t="n"/>
     </row>
     <row r="18">
       <c r="A18" s="1" t="n">
@@ -966,10 +918,7 @@
       <c r="F18" s="0" t="n">
         <v>0</v>
       </c>
-      <c r="G18" s="1">
-        <f>F18*E18</f>
-        <v/>
-      </c>
+      <c r="G18" s="1" t="n"/>
     </row>
     <row r="19">
       <c r="A19" s="1" t="n">
@@ -996,10 +945,7 @@
       <c r="F19" s="0" t="n">
         <v>0</v>
       </c>
-      <c r="G19" s="1">
-        <f>F19*E19</f>
-        <v/>
-      </c>
+      <c r="G19" s="1" t="n"/>
     </row>
     <row r="20">
       <c r="A20" s="1" t="n">
@@ -1026,10 +972,7 @@
       <c r="F20" s="0" t="n">
         <v>0</v>
       </c>
-      <c r="G20" s="1">
-        <f>F20*E20</f>
-        <v/>
-      </c>
+      <c r="G20" s="1" t="n"/>
     </row>
     <row r="21">
       <c r="A21" s="1" t="n">
@@ -1056,10 +999,7 @@
       <c r="F21" s="0" t="n">
         <v>0</v>
       </c>
-      <c r="G21" s="1">
-        <f>F21*E21</f>
-        <v/>
-      </c>
+      <c r="G21" s="1" t="n"/>
     </row>
     <row r="22">
       <c r="A22" s="1" t="n">
@@ -1086,10 +1026,7 @@
       <c r="F22" s="0" t="n">
         <v>0</v>
       </c>
-      <c r="G22" s="1">
-        <f>F22*E22</f>
-        <v/>
-      </c>
+      <c r="G22" s="1" t="n"/>
     </row>
     <row r="23">
       <c r="A23" s="1" t="n">
@@ -1116,10 +1053,7 @@
       <c r="F23" s="0" t="n">
         <v>0</v>
       </c>
-      <c r="G23" s="1">
-        <f>F23*E23</f>
-        <v/>
-      </c>
+      <c r="G23" s="1" t="n"/>
     </row>
     <row r="24">
       <c r="A24" s="1" t="n">
@@ -1146,10 +1080,7 @@
       <c r="F24" s="0" t="n">
         <v>0</v>
       </c>
-      <c r="G24" s="1">
-        <f>F24*E24</f>
-        <v/>
-      </c>
+      <c r="G24" s="1" t="n"/>
     </row>
     <row r="25">
       <c r="A25" s="1" t="n">
@@ -1176,10 +1107,7 @@
       <c r="F25" s="0" t="n">
         <v>0</v>
       </c>
-      <c r="G25" s="1">
-        <f>F25*E25</f>
-        <v/>
-      </c>
+      <c r="G25" s="1" t="n"/>
     </row>
     <row r="26">
       <c r="A26" s="1" t="n">
@@ -1206,10 +1134,7 @@
       <c r="F26" s="0" t="n">
         <v>0</v>
       </c>
-      <c r="G26" s="1">
-        <f>F26*E26</f>
-        <v/>
-      </c>
+      <c r="G26" s="1" t="n"/>
     </row>
     <row r="27">
       <c r="A27" s="1" t="n">
@@ -1236,10 +1161,7 @@
       <c r="F27" s="0" t="n">
         <v>0</v>
       </c>
-      <c r="G27" s="1">
-        <f>F27*E27</f>
-        <v/>
-      </c>
+      <c r="G27" s="1" t="n"/>
     </row>
     <row r="28">
       <c r="A28" s="1" t="n">
@@ -1266,10 +1188,7 @@
       <c r="F28" s="0" t="n">
         <v>0</v>
       </c>
-      <c r="G28" s="1">
-        <f>F28*E28</f>
-        <v/>
-      </c>
+      <c r="G28" s="1" t="n"/>
     </row>
     <row r="29">
       <c r="A29" s="1" t="n">
@@ -1296,10 +1215,7 @@
       <c r="F29" s="0" t="n">
         <v>0</v>
       </c>
-      <c r="G29" s="1">
-        <f>F29*E29</f>
-        <v/>
-      </c>
+      <c r="G29" s="1" t="n"/>
     </row>
     <row r="30">
       <c r="A30" s="1" t="n">
@@ -1326,10 +1242,7 @@
       <c r="F30" s="0" t="n">
         <v>0</v>
       </c>
-      <c r="G30" s="1">
-        <f>F30*E30</f>
-        <v/>
-      </c>
+      <c r="G30" s="1" t="n"/>
     </row>
     <row r="31">
       <c r="A31" s="1" t="n">
@@ -1356,10 +1269,7 @@
       <c r="F31" s="0" t="n">
         <v>0</v>
       </c>
-      <c r="G31" s="1">
-        <f>F31*E31</f>
-        <v/>
-      </c>
+      <c r="G31" s="1" t="n"/>
     </row>
     <row r="32">
       <c r="A32" s="1" t="n">
@@ -1386,10 +1296,7 @@
       <c r="F32" s="0" t="n">
         <v>0</v>
       </c>
-      <c r="G32" s="1">
-        <f>F32*E32</f>
-        <v/>
-      </c>
+      <c r="G32" s="1" t="n"/>
     </row>
     <row r="33">
       <c r="A33" s="1" t="n">
@@ -1416,10 +1323,7 @@
       <c r="F33" s="0" t="n">
         <v>0</v>
       </c>
-      <c r="G33" s="1">
-        <f>F33*E33</f>
-        <v/>
-      </c>
+      <c r="G33" s="1" t="n"/>
     </row>
     <row r="34">
       <c r="A34" s="1" t="n">
@@ -1446,10 +1350,7 @@
       <c r="F34" s="0" t="n">
         <v>0</v>
       </c>
-      <c r="G34" s="1">
-        <f>F34*E34</f>
-        <v/>
-      </c>
+      <c r="G34" s="1" t="n"/>
     </row>
     <row r="35">
       <c r="A35" s="1" t="n">
@@ -1476,10 +1377,7 @@
       <c r="F35" s="0" t="n">
         <v>0</v>
       </c>
-      <c r="G35" s="1">
-        <f>F35*E35</f>
-        <v/>
-      </c>
+      <c r="G35" s="1" t="n"/>
     </row>
     <row r="36">
       <c r="A36" s="1" t="n">
@@ -1506,10 +1404,7 @@
       <c r="F36" s="0" t="n">
         <v>0</v>
       </c>
-      <c r="G36" s="1">
-        <f>F36*E36</f>
-        <v/>
-      </c>
+      <c r="G36" s="1" t="n"/>
     </row>
     <row r="37">
       <c r="A37" s="1" t="n">
@@ -1536,10 +1431,7 @@
       <c r="F37" s="0" t="n">
         <v>0</v>
       </c>
-      <c r="G37" s="1">
-        <f>F37*E37</f>
-        <v/>
-      </c>
+      <c r="G37" s="1" t="n"/>
     </row>
     <row r="38">
       <c r="A38" s="1" t="n">
@@ -1566,10 +1458,7 @@
       <c r="F38" s="0" t="n">
         <v>0</v>
       </c>
-      <c r="G38" s="1">
-        <f>F38*E38</f>
-        <v/>
-      </c>
+      <c r="G38" s="1" t="n"/>
     </row>
     <row r="39">
       <c r="A39" s="1" t="n">
@@ -1596,10 +1485,7 @@
       <c r="F39" s="0" t="n">
         <v>0</v>
       </c>
-      <c r="G39" s="1">
-        <f>F39*E39</f>
-        <v/>
-      </c>
+      <c r="G39" s="1" t="n"/>
     </row>
     <row r="40">
       <c r="A40" s="1" t="n">
@@ -1626,9 +1512,1240 @@
       <c r="F40" s="0" t="n">
         <v>0</v>
       </c>
-      <c r="G40" s="1">
-        <f>F40*E40</f>
-        <v/>
+      <c r="G40" s="1" t="n"/>
+    </row>
+    <row r="41">
+      <c r="A41" s="0" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+      <c r="B41" s="0" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+      <c r="C41" s="0" t="inlineStr">
+        <is>
+          <t>김밥</t>
+        </is>
+      </c>
+      <c r="D41" s="0" t="inlineStr">
+        <is>
+          <t>10000</t>
+        </is>
+      </c>
+      <c r="E41" s="0" t="inlineStr">
+        <is>
+          <t>12줄</t>
+        </is>
+      </c>
+      <c r="F41" s="0" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+      <c r="G41" s="0" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" s="0" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+      <c r="B42" s="0" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+      <c r="C42" s="0" t="inlineStr">
+        <is>
+          <t>짜장면</t>
+        </is>
+      </c>
+      <c r="D42" s="0" t="inlineStr">
+        <is>
+          <t>쟁반</t>
+        </is>
+      </c>
+      <c r="E42" s="0" t="inlineStr">
+        <is>
+          <t>8000</t>
+        </is>
+      </c>
+      <c r="F42" s="0" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+      <c r="G42" s="0" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" s="0" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+      <c r="B43" s="0" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+      <c r="C43" s="0" t="inlineStr">
+        <is>
+          <t>ety</t>
+        </is>
+      </c>
+      <c r="D43" s="0" t="inlineStr">
+        <is>
+          <t>etyh</t>
+        </is>
+      </c>
+      <c r="E43" s="0" t="inlineStr">
+        <is>
+          <t>eth</t>
+        </is>
+      </c>
+      <c r="F43" s="0" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+      <c r="G43" s="0" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" s="0" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+      <c r="B44" s="0" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+      <c r="C44" s="0" t="inlineStr">
+        <is>
+          <t>tyh</t>
+        </is>
+      </c>
+      <c r="D44" s="0" t="inlineStr">
+        <is>
+          <t>tyh</t>
+        </is>
+      </c>
+      <c r="E44" s="0" t="inlineStr">
+        <is>
+          <t>tyh</t>
+        </is>
+      </c>
+      <c r="F44" s="0" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+      <c r="G44" s="0" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" s="0" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+      <c r="B45" s="0" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+      <c r="C45" s="0" t="inlineStr">
+        <is>
+          <t>a</t>
+        </is>
+      </c>
+      <c r="D45" s="0" t="inlineStr">
+        <is>
+          <t>a</t>
+        </is>
+      </c>
+      <c r="E45" s="0" t="inlineStr">
+        <is>
+          <t>a</t>
+        </is>
+      </c>
+      <c r="F45" s="0" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+      <c r="G45" s="0" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" s="0" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+      <c r="B46" s="0" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+      <c r="C46" s="0" t="inlineStr">
+        <is>
+          <t>b</t>
+        </is>
+      </c>
+      <c r="D46" s="0" t="inlineStr">
+        <is>
+          <t>b</t>
+        </is>
+      </c>
+      <c r="E46" s="0" t="inlineStr">
+        <is>
+          <t>b</t>
+        </is>
+      </c>
+      <c r="F46" s="0" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+      <c r="G46" s="0" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" s="0" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+      <c r="B47" s="0" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+      <c r="C47" s="0" t="inlineStr">
+        <is>
+          <t>q</t>
+        </is>
+      </c>
+      <c r="D47" s="0" t="inlineStr">
+        <is>
+          <t>q</t>
+        </is>
+      </c>
+      <c r="E47" s="0" t="inlineStr">
+        <is>
+          <t>q</t>
+        </is>
+      </c>
+      <c r="F47" s="0" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+      <c r="G47" s="0" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" s="0" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+      <c r="B48" s="0" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+      <c r="C48" s="0" t="inlineStr">
+        <is>
+          <t>s</t>
+        </is>
+      </c>
+      <c r="D48" s="0" t="inlineStr">
+        <is>
+          <t>s</t>
+        </is>
+      </c>
+      <c r="E48" s="0" t="inlineStr">
+        <is>
+          <t>s</t>
+        </is>
+      </c>
+      <c r="F48" s="0" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+      <c r="G48" s="0" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" s="0" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+      <c r="B49" s="0" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+      <c r="C49" s="0" t="inlineStr">
+        <is>
+          <t>s</t>
+        </is>
+      </c>
+      <c r="D49" s="0" t="inlineStr">
+        <is>
+          <t>s</t>
+        </is>
+      </c>
+      <c r="E49" s="0" t="inlineStr">
+        <is>
+          <t>s</t>
+        </is>
+      </c>
+      <c r="F49" s="0" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+      <c r="G49" s="0" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" s="0" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+      <c r="B50" s="0" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+      <c r="C50" s="0" t="inlineStr">
+        <is>
+          <t>gg</t>
+        </is>
+      </c>
+      <c r="D50" s="0" t="inlineStr">
+        <is>
+          <t>gg</t>
+        </is>
+      </c>
+      <c r="E50" s="0" t="inlineStr">
+        <is>
+          <t>gg</t>
+        </is>
+      </c>
+      <c r="F50" s="0" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+      <c r="G50" s="0" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" s="0" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+      <c r="B51" s="0" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+      <c r="C51" s="0" t="inlineStr">
+        <is>
+          <t>ggg</t>
+        </is>
+      </c>
+      <c r="D51" s="0" t="inlineStr">
+        <is>
+          <t>ggg</t>
+        </is>
+      </c>
+      <c r="E51" s="0" t="inlineStr">
+        <is>
+          <t>ggg</t>
+        </is>
+      </c>
+      <c r="F51" s="0" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+      <c r="G51" s="0" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" s="0" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+      <c r="B52" s="0" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+      <c r="C52" s="0" t="inlineStr">
+        <is>
+          <t>rrrr</t>
+        </is>
+      </c>
+      <c r="D52" s="0" t="inlineStr">
+        <is>
+          <t>rrr</t>
+        </is>
+      </c>
+      <c r="E52" s="0" t="inlineStr">
+        <is>
+          <t>rrrr</t>
+        </is>
+      </c>
+      <c r="F52" s="0" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+      <c r="G52" s="0" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" s="0" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+      <c r="B53" s="0" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+      <c r="C53" s="0" t="inlineStr"/>
+      <c r="D53" s="0" t="inlineStr"/>
+      <c r="E53" s="0" t="inlineStr"/>
+      <c r="F53" s="0" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+      <c r="G53" s="0" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54" s="0" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+      <c r="B54" s="0" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+      <c r="C54" s="0" t="inlineStr"/>
+      <c r="D54" s="0" t="inlineStr"/>
+      <c r="E54" s="0" t="inlineStr"/>
+      <c r="F54" s="0" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+      <c r="G54" s="0" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+    </row>
+    <row r="55">
+      <c r="A55" s="0" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+      <c r="B55" s="0" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+      <c r="C55" s="0" t="inlineStr">
+        <is>
+          <t>dfv</t>
+        </is>
+      </c>
+      <c r="D55" s="0" t="inlineStr">
+        <is>
+          <t>vdfv</t>
+        </is>
+      </c>
+      <c r="E55" s="0" t="inlineStr">
+        <is>
+          <t>dfvd</t>
+        </is>
+      </c>
+      <c r="F55" s="0" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+      <c r="G55" s="0" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+    </row>
+    <row r="56">
+      <c r="A56" s="0" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+      <c r="B56" s="0" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+      <c r="C56" s="0" t="inlineStr">
+        <is>
+          <t>fsgb</t>
+        </is>
+      </c>
+      <c r="D56" s="0" t="inlineStr">
+        <is>
+          <t>bggg</t>
+        </is>
+      </c>
+      <c r="E56" s="0" t="inlineStr">
+        <is>
+          <t>sbg</t>
+        </is>
+      </c>
+      <c r="F56" s="0" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+      <c r="G56" s="0" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+    </row>
+    <row r="57">
+      <c r="A57" s="0" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+      <c r="B57" s="0" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+      <c r="C57" s="0" t="inlineStr">
+        <is>
+          <t>wwww</t>
+        </is>
+      </c>
+      <c r="D57" s="0" t="inlineStr">
+        <is>
+          <t>wwww</t>
+        </is>
+      </c>
+      <c r="E57" s="0" t="inlineStr">
+        <is>
+          <t>wwww</t>
+        </is>
+      </c>
+      <c r="F57" s="0" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+      <c r="G57" s="0" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+    </row>
+    <row r="58">
+      <c r="A58" s="0" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+      <c r="B58" s="0" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+      <c r="C58" s="0" t="inlineStr">
+        <is>
+          <t>hwrth</t>
+        </is>
+      </c>
+      <c r="D58" s="0" t="inlineStr">
+        <is>
+          <t>wrtwwwthr</t>
+        </is>
+      </c>
+      <c r="E58" s="0" t="inlineStr">
+        <is>
+          <t>rwthwrth</t>
+        </is>
+      </c>
+      <c r="F58" s="0" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+      <c r="G58" s="0" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+    </row>
+    <row r="59">
+      <c r="A59" s="0" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+      <c r="B59" s="0" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+      <c r="C59" s="0" t="inlineStr">
+        <is>
+          <t>jjjy</t>
+        </is>
+      </c>
+      <c r="D59" s="0" t="inlineStr">
+        <is>
+          <t>jyjyj</t>
+        </is>
+      </c>
+      <c r="E59" s="0" t="inlineStr">
+        <is>
+          <t>jjjy</t>
+        </is>
+      </c>
+      <c r="F59" s="0" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+      <c r="G59" s="0" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+    </row>
+    <row r="60">
+      <c r="A60" s="0" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+      <c r="B60" s="0" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+      <c r="C60" s="0" t="inlineStr">
+        <is>
+          <t>weg</t>
+        </is>
+      </c>
+      <c r="D60" s="0" t="inlineStr">
+        <is>
+          <t>weg</t>
+        </is>
+      </c>
+      <c r="E60" s="0" t="inlineStr">
+        <is>
+          <t>weg</t>
+        </is>
+      </c>
+      <c r="F60" s="0" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+      <c r="G60" s="0" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+    </row>
+    <row r="61">
+      <c r="A61" s="0" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+      <c r="B61" s="0" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+      <c r="C61" s="0" t="inlineStr">
+        <is>
+          <t>감튀</t>
+        </is>
+      </c>
+      <c r="D61" s="0" t="inlineStr">
+        <is>
+          <t>개</t>
+        </is>
+      </c>
+      <c r="E61" s="0" t="inlineStr">
+        <is>
+          <t>3300</t>
+        </is>
+      </c>
+      <c r="F61" s="0" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+      <c r="G61" s="0" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+    </row>
+    <row r="62">
+      <c r="A62" s="0" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+      <c r="B62" s="0" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+      <c r="C62" s="0" t="inlineStr">
+        <is>
+          <t>ㅈㄹㅈㄷㄹ</t>
+        </is>
+      </c>
+      <c r="D62" s="0" t="inlineStr">
+        <is>
+          <t>ㄹㅈㄷㄹㅈㄷㄹ</t>
+        </is>
+      </c>
+      <c r="E62" s="0" t="inlineStr">
+        <is>
+          <t>ㄹㅈㄷㄹㅈㄷㄹ</t>
+        </is>
+      </c>
+      <c r="F62" s="0" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+      <c r="G62" s="0" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+    </row>
+    <row r="63">
+      <c r="A63" s="0" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+      <c r="B63" s="0" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+      <c r="C63" s="0" t="inlineStr">
+        <is>
+          <t>ㅂㅂㅂ</t>
+        </is>
+      </c>
+      <c r="D63" s="0" t="inlineStr">
+        <is>
+          <t>ㅂㅂㅂㅂ</t>
+        </is>
+      </c>
+      <c r="E63" s="0" t="inlineStr">
+        <is>
+          <t>ㅂㅂㅂㅂ</t>
+        </is>
+      </c>
+      <c r="F63" s="0" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+      <c r="G63" s="0" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+    </row>
+    <row r="64">
+      <c r="A64" s="0" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+      <c r="B64" s="0" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+      <c r="C64" s="0" t="inlineStr">
+        <is>
+          <t>ㄹㄹㄹ</t>
+        </is>
+      </c>
+      <c r="D64" s="0" t="inlineStr">
+        <is>
+          <t>ㄹㄹㄹ</t>
+        </is>
+      </c>
+      <c r="E64" s="0" t="inlineStr">
+        <is>
+          <t>ㄹㄹㄹㄹ</t>
+        </is>
+      </c>
+      <c r="F64" s="0" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+      <c r="G64" s="0" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+    </row>
+    <row r="65">
+      <c r="A65" s="0" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+      <c r="B65" s="0" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+      <c r="C65" s="0" t="inlineStr">
+        <is>
+          <t>ㄹㅂㅈㄷㄹㅈ</t>
+        </is>
+      </c>
+      <c r="D65" s="0" t="inlineStr">
+        <is>
+          <t>ㄹㅈㄷㄹ</t>
+        </is>
+      </c>
+      <c r="E65" s="0" t="inlineStr">
+        <is>
+          <t>ㅈㄹㅂㅈㄷㄹ</t>
+        </is>
+      </c>
+      <c r="F65" s="0" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+      <c r="G65" s="0" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+    </row>
+    <row r="66">
+      <c r="A66" s="0" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+      <c r="B66" s="0" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+      <c r="C66" s="0" t="inlineStr">
+        <is>
+          <t>피클</t>
+        </is>
+      </c>
+      <c r="D66" s="0" t="inlineStr">
+        <is>
+          <t>ㄹㄹㄹ</t>
+        </is>
+      </c>
+      <c r="E66" s="0" t="inlineStr">
+        <is>
+          <t>클ㄹㄹ</t>
+        </is>
+      </c>
+      <c r="F66" s="0" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+      <c r="G66" s="0" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+    </row>
+    <row r="67">
+      <c r="A67" s="0" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+      <c r="B67" s="0" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+      <c r="C67" s="0" t="inlineStr">
+        <is>
+          <t>ㅈㅂㄷㄹ</t>
+        </is>
+      </c>
+      <c r="D67" s="0" t="inlineStr">
+        <is>
+          <t>ㄹㅂㅈㄷㄹ</t>
+        </is>
+      </c>
+      <c r="E67" s="0" t="inlineStr">
+        <is>
+          <t>ㄹㅂㅈㄷㄹ</t>
+        </is>
+      </c>
+      <c r="F67" s="0" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+      <c r="G67" s="0" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+    </row>
+    <row r="68">
+      <c r="A68" s="0" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+      <c r="B68" s="0" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+      <c r="C68" s="0" t="inlineStr">
+        <is>
+          <t>ㅂㅈㄷㄹ</t>
+        </is>
+      </c>
+      <c r="D68" s="0" t="inlineStr">
+        <is>
+          <t>ㄹㅈㅂㄷㄹ</t>
+        </is>
+      </c>
+      <c r="E68" s="0" t="inlineStr">
+        <is>
+          <t>ㄹㅂㅈㄷㄹ</t>
+        </is>
+      </c>
+      <c r="F68" s="0" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+      <c r="G68" s="0" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+    </row>
+    <row r="69">
+      <c r="A69" s="0" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+      <c r="B69" s="0" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+      <c r="C69" s="0" t="inlineStr">
+        <is>
+          <t>ㅁㄴㅇㄹ</t>
+        </is>
+      </c>
+      <c r="D69" s="0" t="inlineStr">
+        <is>
+          <t>ㄹㄴㅁㅇㄹ</t>
+        </is>
+      </c>
+      <c r="E69" s="0" t="inlineStr">
+        <is>
+          <t>ㄹㅁㄴㅇㄹ</t>
+        </is>
+      </c>
+      <c r="F69" s="0" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+      <c r="G69" s="0" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+    </row>
+    <row r="70">
+      <c r="A70" s="0" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+      <c r="B70" s="0" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+      <c r="C70" s="0" t="inlineStr">
+        <is>
+          <t>ㄹㄹㄹ</t>
+        </is>
+      </c>
+      <c r="D70" s="0" t="inlineStr">
+        <is>
+          <t>ㄹㄹㄹ</t>
+        </is>
+      </c>
+      <c r="E70" s="0" t="inlineStr">
+        <is>
+          <t>ㄹㄹㄹㄹ</t>
+        </is>
+      </c>
+      <c r="F70" s="0" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+      <c r="G70" s="0" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+    </row>
+    <row r="71">
+      <c r="A71" s="0" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+      <c r="B71" s="0" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+      <c r="C71" s="0" t="inlineStr">
+        <is>
+          <t>ㄷㄱ소</t>
+        </is>
+      </c>
+      <c r="D71" s="0" t="inlineStr">
+        <is>
+          <t>솓ㄱ소</t>
+        </is>
+      </c>
+      <c r="E71" s="0" t="inlineStr">
+        <is>
+          <t>솓ㄱ소</t>
+        </is>
+      </c>
+      <c r="F71" s="0" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+      <c r="G71" s="0" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+    </row>
+    <row r="72">
+      <c r="A72" s="0" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+      <c r="B72" s="0" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+      <c r="C72" s="0" t="inlineStr">
+        <is>
+          <t>888888</t>
+        </is>
+      </c>
+      <c r="D72" s="0" t="inlineStr">
+        <is>
+          <t>8888888</t>
+        </is>
+      </c>
+      <c r="E72" s="0" t="inlineStr">
+        <is>
+          <t>8888888</t>
+        </is>
+      </c>
+      <c r="F72" s="0" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+      <c r="G72" s="0" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+    </row>
+    <row r="73">
+      <c r="A73" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+      <c r="B73" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+      <c r="C73" t="inlineStr">
+        <is>
+          <t>fff</t>
+        </is>
+      </c>
+      <c r="D73" t="inlineStr">
+        <is>
+          <t>fff</t>
+        </is>
+      </c>
+      <c r="E73" t="inlineStr">
+        <is>
+          <t>fff</t>
+        </is>
+      </c>
+      <c r="F73" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+      <c r="G73" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+    </row>
+    <row r="74">
+      <c r="A74" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+      <c r="B74" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+      <c r="C74" t="inlineStr">
+        <is>
+          <t>ssss</t>
+        </is>
+      </c>
+      <c r="D74" t="inlineStr">
+        <is>
+          <t>ssss</t>
+        </is>
+      </c>
+      <c r="E74" t="inlineStr">
+        <is>
+          <t>ssss</t>
+        </is>
+      </c>
+      <c r="F74" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+      <c r="G74" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
+        </is>
       </c>
     </row>
   </sheetData>

</xml_diff>